<commit_message>
changement du tableau de synthèse
</commit_message>
<xml_diff>
--- a/public/fichiers/tableausynthese.xlsx
+++ b/public/fichiers/tableausynthese.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cours\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D22BC4-8DC3-4715-8EFA-BA04790CC28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C278193F-722E-43B9-BEB2-938F6D6F9A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -176,6 +176,46 @@
     <t>Centre de formation : Lycée Carcouët</t>
   </si>
   <si>
+    <t>SESSION 2025</t>
+  </si>
+  <si>
+    <t>AP4 : Conception d'une application web de gestion de tâches (PHP, SQL)</t>
+  </si>
+  <si>
+    <t>TP Installation et configuration d'un outil de gestion de par cet de configurations (GLPI)</t>
+  </si>
+  <si>
+    <t>Planification des tâches avec Asana pour en déterminer la durée</t>
+  </si>
+  <si>
+    <t>Réalisation de documentations. de spécifications pour faciliter l'utilisation (NAS de l'entreprise)</t>
+  </si>
+  <si>
+    <t>Réunions pour décrire les tâches réalisées chaque journée (SCRUM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réponse à demandes d'assistance via des tickets sur Asana </t>
+  </si>
+  <si>
+    <t>Réalisation de documentations pour l'entreprise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Déploiements d'applications sur serveurs de tests/production </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veille technologique </t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rélisation d'un compte LinkedIn
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création d'un Portfolio </t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Adresse URL </t>
     </r>
@@ -183,52 +223,12 @@
       <rPr>
         <b/>
         <sz val="18"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">du portfolio : </t>
+      <t>du portfolio : https://pablo-leparoux-portfolio.netlify.app/</t>
     </r>
-  </si>
-  <si>
-    <t>SESSION 2025</t>
-  </si>
-  <si>
-    <t>AP4 : Conception d'une application web de gestion de tâches (PHP, SQL)</t>
-  </si>
-  <si>
-    <t>TP Installation et configuration d'un outil de gestion de par cet de configurations (GLPI)</t>
-  </si>
-  <si>
-    <t>Planification des tâches avec Asana pour en déterminer la durée</t>
-  </si>
-  <si>
-    <t>Réalisation de documentations. de spécifications pour faciliter l'utilisation (NAS de l'entreprise)</t>
-  </si>
-  <si>
-    <t>Réunions pour décrire les tâches réalisées chaque journée (SCRUM)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Réponse à demandes d'assistance via des tickets sur Asana </t>
-  </si>
-  <si>
-    <t>Réalisation de documentations pour l'entreprise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Déploiements d'applications sur serveurs de tests/production </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Veille technologique </t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rélisation d'un compte LinkedIn
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Création d'un Portfolio </t>
   </si>
 </sst>
 </file>
@@ -304,7 +304,7 @@
     <font>
       <b/>
       <sz val="18"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1268,8 +1268,8 @@
   </sheetPr>
   <dimension ref="A1:AQ85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="66" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="66" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1291,7 +1291,7 @@
       <c r="E1" s="28"/>
       <c r="F1" s="28"/>
       <c r="G1" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H1" s="29"/>
     </row>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="5" spans="1:43" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="52" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="B5" s="53"/>
       <c r="C5" s="53"/>
@@ -1645,7 +1645,7 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>24</v>
@@ -1698,10 +1698,10 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -1749,7 +1749,7 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>23</v>
@@ -1802,7 +1802,7 @@
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>23</v>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>32</v>
@@ -2239,7 +2239,7 @@
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="26"/>
       <c r="C24" s="9" t="s">
@@ -2339,7 +2339,7 @@
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="9"/>
@@ -2435,7 +2435,7 @@
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28" s="25" t="s">
         <v>33</v>
@@ -2639,7 +2639,7 @@
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B32" s="26"/>
       <c r="C32" s="9"/>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="34" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B34" s="26"/>
       <c r="C34" s="21" t="s">
@@ -2837,7 +2837,7 @@
     </row>
     <row r="36" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" s="26"/>
       <c r="C36" s="21" t="s">
@@ -2886,7 +2886,7 @@
     </row>
     <row r="37" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B37" s="26"/>
       <c r="C37" s="21"/>

</xml_diff>